<commit_message>
deactivate button when clicked on
</commit_message>
<xml_diff>
--- a/eval_conscience_data.xlsx
+++ b/eval_conscience_data.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I8"/>
+  <dimension ref="A1:J27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -486,6 +486,11 @@
           <t>commentaire</t>
         </is>
       </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>temps_validation</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="2" t="n">
@@ -527,6 +532,7 @@
           <t>zeerf</t>
         </is>
       </c>
+      <c r="J2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" s="2" t="n">
@@ -568,6 +574,7 @@
           <t>reea</t>
         </is>
       </c>
+      <c r="J3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" s="2" t="n">
@@ -609,6 +616,7 @@
           <t>ee</t>
         </is>
       </c>
+      <c r="J4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" s="2" t="n">
@@ -646,6 +654,7 @@
         </is>
       </c>
       <c r="I5" t="inlineStr"/>
+      <c r="J5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" s="2" t="n">
@@ -687,6 +696,7 @@
           <t>eeert</t>
         </is>
       </c>
+      <c r="J6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" s="2" t="n">
@@ -728,9 +738,10 @@
           <t>ddd</t>
         </is>
       </c>
+      <c r="J7" t="inlineStr"/>
     </row>
     <row r="8">
-      <c r="A8" s="3" t="n">
+      <c r="A8" s="2" t="n">
         <v>45680</v>
       </c>
       <c r="B8" t="inlineStr">
@@ -768,6 +779,819 @@
         <is>
           <t>peut etre</t>
         </is>
+      </c>
+      <c r="J8" t="inlineStr"/>
+    </row>
+    <row r="9">
+      <c r="A9" s="2" t="n">
+        <v>45716</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>03:03</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>ttttz</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>MK</t>
+        </is>
+      </c>
+      <c r="E9" t="n">
+        <v>0.38</v>
+      </c>
+      <c r="F9" t="n">
+        <v>-0.31</v>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>aaa</t>
+        </is>
+      </c>
+      <c r="J9" s="2" t="n">
+        <v>45716.41619204861</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="2" t="n">
+        <v>45734</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>05:06</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>mat6</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>MK</t>
+        </is>
+      </c>
+      <c r="E10" t="n">
+        <v>-0.19</v>
+      </c>
+      <c r="F10" t="n">
+        <v>0.36</v>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr"/>
+      <c r="J10" s="2" t="n">
+        <v>45734.60008083333</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="2" t="n">
+        <v>45734</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>20:56</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>mat9</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>IDE</t>
+        </is>
+      </c>
+      <c r="E11" t="n">
+        <v>-0.37</v>
+      </c>
+      <c r="F11" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr"/>
+      <c r="J11" s="2" t="n">
+        <v>45734.60044688657</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="2" t="n">
+        <v>45734</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>06:02</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>jhg</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>AS</t>
+        </is>
+      </c>
+      <c r="E12" t="n">
+        <v>-0.48</v>
+      </c>
+      <c r="F12" t="n">
+        <v>0.34</v>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="I12" t="inlineStr"/>
+      <c r="J12" s="2" t="n">
+        <v>45734.60465787037</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="2" t="n">
+        <v>45762</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>02:04</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>testbut</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>MK</t>
+        </is>
+      </c>
+      <c r="E13" t="n">
+        <v>0</v>
+      </c>
+      <c r="F13" t="n">
+        <v>0</v>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>butbut</t>
+        </is>
+      </c>
+      <c r="J13" s="2" t="n">
+        <v>45762.43662241898</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="2" t="n">
+        <v>45762</v>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>02:04</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>testbut</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>MK</t>
+        </is>
+      </c>
+      <c r="E14" t="n">
+        <v>0</v>
+      </c>
+      <c r="F14" t="n">
+        <v>0</v>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t>butbut</t>
+        </is>
+      </c>
+      <c r="J14" s="2" t="n">
+        <v>45762.43664268518</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="2" t="n">
+        <v>45762</v>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>02:04</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>testbut</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>MK</t>
+        </is>
+      </c>
+      <c r="E15" t="n">
+        <v>0</v>
+      </c>
+      <c r="F15" t="n">
+        <v>0</v>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="I15" t="inlineStr">
+        <is>
+          <t>butbut</t>
+        </is>
+      </c>
+      <c r="J15" s="2" t="n">
+        <v>45762.43665787037</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="2" t="n">
+        <v>45762</v>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>01:02</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>testbut2</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>MK</t>
+        </is>
+      </c>
+      <c r="E16" t="n">
+        <v>0</v>
+      </c>
+      <c r="F16" t="n">
+        <v>0</v>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="I16" t="inlineStr">
+        <is>
+          <t>butbut2</t>
+        </is>
+      </c>
+      <c r="J16" s="2" t="n">
+        <v>45762.44171180556</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="2" t="n">
+        <v>45762</v>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>01:02</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>testbut2</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>MK</t>
+        </is>
+      </c>
+      <c r="E17" t="n">
+        <v>0</v>
+      </c>
+      <c r="F17" t="n">
+        <v>0</v>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="I17" t="inlineStr">
+        <is>
+          <t>butbut2</t>
+        </is>
+      </c>
+      <c r="J17" s="2" t="n">
+        <v>45762.44173680556</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="2" t="n">
+        <v>45762</v>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>01:02</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>testbut2</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>MK</t>
+        </is>
+      </c>
+      <c r="E18" t="n">
+        <v>0</v>
+      </c>
+      <c r="F18" t="n">
+        <v>0</v>
+      </c>
+      <c r="G18" t="inlineStr"/>
+      <c r="H18" t="inlineStr"/>
+      <c r="I18" t="inlineStr"/>
+      <c r="J18" s="2" t="n">
+        <v>45762.44176215278</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="2" t="n">
+        <v>45762</v>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>02:03</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>testbut3</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>Proche</t>
+        </is>
+      </c>
+      <c r="E19" t="n">
+        <v>0</v>
+      </c>
+      <c r="F19" t="n">
+        <v>0</v>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="I19" t="inlineStr">
+        <is>
+          <t>but3</t>
+        </is>
+      </c>
+      <c r="J19" s="2" t="n">
+        <v>45762.44206026621</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="2" t="n">
+        <v>45762</v>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>02:03</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>testbut3</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>Proche</t>
+        </is>
+      </c>
+      <c r="E20" t="n">
+        <v>0</v>
+      </c>
+      <c r="F20" t="n">
+        <v>0</v>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="I20" t="inlineStr">
+        <is>
+          <t>but3</t>
+        </is>
+      </c>
+      <c r="J20" s="2" t="n">
+        <v>45762.44206666667</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="2" t="n">
+        <v>45762</v>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>04:03</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>but4</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>Proche</t>
+        </is>
+      </c>
+      <c r="E21" t="n">
+        <v>0</v>
+      </c>
+      <c r="F21" t="n">
+        <v>0</v>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="I21" t="inlineStr">
+        <is>
+          <t>but4</t>
+        </is>
+      </c>
+      <c r="J21" s="2" t="n">
+        <v>45762.442665625</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="2" t="n">
+        <v>45762</v>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>04:03</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>but4</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>Proche</t>
+        </is>
+      </c>
+      <c r="E22" t="n">
+        <v>0</v>
+      </c>
+      <c r="F22" t="n">
+        <v>0</v>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="I22" t="inlineStr">
+        <is>
+          <t>but4</t>
+        </is>
+      </c>
+      <c r="J22" s="2" t="n">
+        <v>45762.44266758102</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="2" t="n">
+        <v>45762</v>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>03:03</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>but5</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>MK</t>
+        </is>
+      </c>
+      <c r="E23" t="n">
+        <v>0</v>
+      </c>
+      <c r="F23" t="n">
+        <v>0</v>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="H23" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="I23" t="inlineStr">
+        <is>
+          <t>but5</t>
+        </is>
+      </c>
+      <c r="J23" s="2" t="n">
+        <v>45762.44375712963</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="2" t="n">
+        <v>45762</v>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>02:01</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>but6</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>MK</t>
+        </is>
+      </c>
+      <c r="E24" t="n">
+        <v>0</v>
+      </c>
+      <c r="F24" t="n">
+        <v>0</v>
+      </c>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="H24" t="inlineStr">
+        <is>
+          <t>OUI</t>
+        </is>
+      </c>
+      <c r="I24" t="inlineStr">
+        <is>
+          <t>butbut6</t>
+        </is>
+      </c>
+      <c r="J24" s="2" t="n">
+        <v>45762.4518687963</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="2" t="n">
+        <v>45762</v>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>03:02</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>but7</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>AS</t>
+        </is>
+      </c>
+      <c r="E25" t="n">
+        <v>0</v>
+      </c>
+      <c r="F25" t="n">
+        <v>0</v>
+      </c>
+      <c r="G25" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="H25" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="I25" t="inlineStr">
+        <is>
+          <t>btu77</t>
+        </is>
+      </c>
+      <c r="J25" s="2" t="n">
+        <v>45762.45207097222</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="2" t="n">
+        <v>45762</v>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>04:04</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>but8</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>Proche</t>
+        </is>
+      </c>
+      <c r="E26" t="n">
+        <v>0</v>
+      </c>
+      <c r="F26" t="n">
+        <v>0</v>
+      </c>
+      <c r="G26" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="H26" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="I26" t="inlineStr">
+        <is>
+          <t>but8</t>
+        </is>
+      </c>
+      <c r="J26" s="2" t="n">
+        <v>45762.45309504629</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="3" t="n">
+        <v>45762</v>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>02:03</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>but9</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>IDE</t>
+        </is>
+      </c>
+      <c r="E27" t="n">
+        <v>0</v>
+      </c>
+      <c r="F27" t="n">
+        <v>0</v>
+      </c>
+      <c r="G27" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="H27" t="inlineStr">
+        <is>
+          <t>NON</t>
+        </is>
+      </c>
+      <c r="I27" t="inlineStr">
+        <is>
+          <t>but9</t>
+        </is>
+      </c>
+      <c r="J27" s="2" t="n">
+        <v>45762.45327601706</v>
       </c>
     </row>
   </sheetData>

</xml_diff>